<commit_message>
loginPageTest has been updated
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/ecommerce/testdata/LoginStatus.xlsx
+++ b/src/main/java/com/qa/ecommerce/testdata/LoginStatus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -77,7 +77,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,6 +88,16 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
       </patternFill>
     </fill>
     <fill>
@@ -184,7 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -196,6 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -495,6 +506,7 @@
     <col min="8" max="8" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -528,6 +540,9 @@
       <c r="J1" t="s" s="10">
         <v>8</v>
       </c>
+      <c r="K1" t="s" s="11">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -560,6 +575,9 @@
       <c r="J2" t="s">
         <v>9</v>
       </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -592,6 +610,9 @@
       <c r="J3" t="s">
         <v>9</v>
       </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -624,6 +645,9 @@
       <c r="J4" t="s">
         <v>10</v>
       </c>
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -653,6 +677,9 @@
       <c r="J5" t="s">
         <v>10</v>
       </c>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -680,6 +707,9 @@
         <v>10</v>
       </c>
       <c r="J6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated thread local driver
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/ecommerce/testdata/LoginStatus.xlsx
+++ b/src/main/java/com/qa/ecommerce/testdata/LoginStatus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -77,7 +77,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="21">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,6 +88,16 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
       </patternFill>
     </fill>
     <fill>
@@ -194,7 +204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -207,6 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -507,6 +518,7 @@
     <col min="9" max="9" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -543,6 +555,9 @@
       <c r="K1" t="s" s="11">
         <v>8</v>
       </c>
+      <c r="L1" t="s" s="12">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -578,6 +593,9 @@
       <c r="K2" t="s">
         <v>9</v>
       </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -613,6 +631,9 @@
       <c r="K3" t="s">
         <v>9</v>
       </c>
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -648,6 +669,9 @@
       <c r="K4" t="s">
         <v>10</v>
       </c>
+      <c r="L4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
@@ -680,6 +704,9 @@
       <c r="K5" t="s">
         <v>10</v>
       </c>
+      <c r="L5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -710,6 +737,9 @@
         <v>10</v>
       </c>
       <c r="K6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>